<commit_message>
Course preparation - Split lecture 12 into 2 - data formatting and formulas
</commit_message>
<xml_diff>
--- a/resources/lecture10.xlsx
+++ b/resources/lecture10.xlsx
@@ -188,6 +188,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" ref="A1:D11" displayName="TABLEONE" name="TABLEONE">
+  <autoFilter ref="A1:D11"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -200,6 +201,7 @@
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" ref="A100:D110" displayName="TABLE_9" name="TABLE_9">
+  <autoFilter ref="A100:D110"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -212,6 +214,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" ref="A12:D22" displayName="TABLE_1" name="TABLE_1">
+  <autoFilter ref="A12:D22"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -224,6 +227,7 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" ref="A23:D33" displayName="TABLE_2" name="TABLE_2">
+  <autoFilter ref="A23:D33"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -236,6 +240,7 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" ref="A34:D44" displayName="TABLE_3" name="TABLE_3">
+  <autoFilter ref="A34:D44"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -248,6 +253,7 @@
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" ref="A45:D55" displayName="TABLE_4" name="TABLE_4">
+  <autoFilter ref="A45:D55"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -260,6 +266,7 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" ref="A56:D66" displayName="TABLE_5" name="TABLE_5">
+  <autoFilter ref="A56:D66"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -272,6 +279,7 @@
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" ref="A67:D77" displayName="TABLE_6" name="TABLE_6">
+  <autoFilter ref="A67:D77"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -284,6 +292,7 @@
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" ref="A78:D88" displayName="TABLE_7" name="TABLE_7">
+  <autoFilter ref="A78:D88"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>
@@ -296,6 +305,7 @@
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" ref="A89:D99" displayName="TABLE_8" name="TABLE_8">
+  <autoFilter ref="A89:D99"/>
   <tableColumns count="4">
     <tableColumn name="Column 1" id="1"/>
     <tableColumn name="Column 2" id="2"/>

</xml_diff>